<commit_message>
AR: update of presentation
</commit_message>
<xml_diff>
--- a/Profiling/PainAnalysis.xlsx
+++ b/Profiling/PainAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\RealmOfTheMadAdam\Profiling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92734CC2-061E-4CF0-A616-D43EB89285D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA2770E-7766-45D1-A5D6-1BDD03F9704B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8E89F3B8-11B8-4E0D-80C8-FC552A892173}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8E89F3B8-11B8-4E0D-80C8-FC552A892173}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="41">
   <si>
     <t>NumEntities</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>Avg Frame Time (MS):</t>
+  </si>
+  <si>
+    <t>Physics System Update (MS):</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1063,7 @@
                   <c:v>Avg Frame Time (MS):</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>AI System Update (MS):</c:v>
+                  <c:v>Physics System Update (MS):</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1119,7 +1122,7 @@
                   <c:v>Avg Frame Time (MS):</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>AI System Update (MS):</c:v>
+                  <c:v>Physics System Update (MS):</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6240,7 +6243,7 @@
   <dimension ref="B4:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6264,7 +6267,7 @@
         <v>39</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>